<commit_message>
Completed up to Model Validation
</commit_message>
<xml_diff>
--- a/TIMESHEET.xlsx
+++ b/TIMESHEET.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\night\repo\school\EGR491-PYMLDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE737B7-2F6D-44E7-83CB-1C035FA51ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C4C1DC-8C1C-41A5-B894-D3C6F6C44F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="1920" windowWidth="21600" windowHeight="11775" xr2:uid="{1FF97693-AB88-40F2-8219-3AFFDC5F630D}"/>
+    <workbookView xWindow="34755" yWindow="3330" windowWidth="21600" windowHeight="11775" xr2:uid="{1FF97693-AB88-40F2-8219-3AFFDC5F630D}"/>
   </bookViews>
   <sheets>
-    <sheet name="IN-DIRECT" sheetId="1" r:id="rId1"/>
+    <sheet name="DIRECT" sheetId="1" r:id="rId1"/>
+    <sheet name="INDIRECT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +68,30 @@
   </si>
   <si>
     <t>Completed P4</t>
+  </si>
+  <si>
+    <t>Overview of P5</t>
+  </si>
+  <si>
+    <t>Responding to Charlie Kendall's questions on basemap</t>
+  </si>
+  <si>
+    <t>Listening to and Replying to Rozen Dixons Discussion on Data Visualization</t>
+  </si>
+  <si>
+    <t>Reviewing/Replying to comments on Discusions</t>
+  </si>
+  <si>
+    <t>Discusion with Nelson about course</t>
+  </si>
+  <si>
+    <t>Review of Grades</t>
+  </si>
+  <si>
+    <t>Wriing intro to ML</t>
+  </si>
+  <si>
+    <t>Wrote on Basics of Scikit Learn</t>
   </si>
 </sst>
 </file>
@@ -121,9 +146,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -145,15 +179,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}" name="Table1" displayName="Table1" ref="A2:C8" totalsRowCount="1">
-  <autoFilter ref="A2:C7" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}" name="Table1" displayName="Table1" ref="A2:C12" totalsRowCount="1">
+  <autoFilter ref="A2:C11" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B4">
     <sortCondition ref="A2:A4"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D6CD45C0-A9A3-4101-813C-860AB1BD326B}" name="Date" totalsRowLabel="Total" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F5F6D275-C77E-41FC-86B5-5074EB217CB4}" name="Time" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D6CD45C0-A9A3-4101-813C-860AB1BD326B}" name="Date" totalsRowLabel="Total" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F5F6D275-C77E-41FC-86B5-5074EB217CB4}" name="Time" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="0"/>
     <tableColumn id="4" xr3:uid="{4FD6A4AF-F8A1-4E0C-9307-791B00B68F98}" name="Use"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9B47FC4-C787-45F6-8801-CA6948D5BA02}" name="Table13" displayName="Table13" ref="A3:C10" totalsRowCount="1">
+  <autoFilter ref="A3:C9" xr:uid="{C9B47FC4-C787-45F6-8801-CA6948D5BA02}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B5">
+    <sortCondition ref="A2:A4"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{533D99C6-4402-40E0-9D6E-6B8A54D3E4E6}" name="Date" totalsRowLabel="Total" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{F6E9EF30-8D46-4BF3-9220-540D3BCA5D04}" name="Time" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{2B6B56BA-097E-40E4-A54D-BA5B74655C18}" name="Use"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -456,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6B472D-D214-4103-B0BB-1AAE529850D5}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,14 +542,14 @@
         <v>5</v>
       </c>
       <c r="G2" s="3">
-        <v>0.31388888888888888</v>
+        <v>0.76180555555555562</v>
       </c>
       <c r="H2" s="4">
-        <v>0.39652777777777781</v>
+        <v>0.82500000000000007</v>
       </c>
       <c r="I2" s="2">
         <f>HOUR(H2-G2)*60 + MINUTE(H2-G2)</f>
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -559,12 +608,56 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1">
+        <v>44366</v>
+      </c>
+      <c r="B8" s="2">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B9" s="2">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B11" s="2">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B12" s="2">
         <f>SUBTOTAL(109,Table1[Time])</f>
-        <v>495</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -574,4 +667,99 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA55D96-8673-42E1-9C36-AF4E023AC519}">
+  <dimension ref="A3:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="67" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44366</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44366</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44003</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <f>SUBTOTAL(109,Table13[Time])</f>
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates did indepth section
</commit_message>
<xml_diff>
--- a/TIMESHEET.xlsx
+++ b/TIMESHEET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\night\repo\school\EGR491-PYMLDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C4C1DC-8C1C-41A5-B894-D3C6F6C44F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C477A97F-4358-4268-8DA8-5982D9A21EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34755" yWindow="3330" windowWidth="21600" windowHeight="11775" xr2:uid="{1FF97693-AB88-40F2-8219-3AFFDC5F630D}"/>
+    <workbookView xWindow="34755" yWindow="3330" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{1FF97693-AB88-40F2-8219-3AFFDC5F630D}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Wrote on Basics of Scikit Learn</t>
+  </si>
+  <si>
+    <t>Trying to understand model validation/Writing section on it</t>
+  </si>
+  <si>
+    <t>Short Discusion with Nelson about progress</t>
+  </si>
+  <si>
+    <t>Making/Checking discusion about dicrepencies with text in python</t>
   </si>
 </sst>
 </file>
@@ -179,14 +188,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}" name="Table1" displayName="Table1" ref="A2:C12" totalsRowCount="1">
-  <autoFilter ref="A2:C11" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}" name="Table1" displayName="Table1" ref="A2:C13" totalsRowCount="1">
+  <autoFilter ref="A2:C12" xr:uid="{ED2B78F6-5F67-48D4-9C08-7EE579E1709F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B4">
     <sortCondition ref="A2:A4"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D6CD45C0-A9A3-4101-813C-860AB1BD326B}" name="Date" totalsRowLabel="Total" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F5F6D275-C77E-41FC-86B5-5074EB217CB4}" name="Time" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F5F6D275-C77E-41FC-86B5-5074EB217CB4}" name="Time" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1"/>
     <tableColumn id="4" xr3:uid="{4FD6A4AF-F8A1-4E0C-9307-791B00B68F98}" name="Use"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -201,7 +210,7 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{533D99C6-4402-40E0-9D6E-6B8A54D3E4E6}" name="Date" totalsRowLabel="Total" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F6E9EF30-8D46-4BF3-9220-540D3BCA5D04}" name="Time" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F6E9EF30-8D46-4BF3-9220-540D3BCA5D04}" name="Time" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0"/>
     <tableColumn id="4" xr3:uid="{2B6B56BA-097E-40E4-A54D-BA5B74655C18}" name="Use"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -505,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6B472D-D214-4103-B0BB-1AAE529850D5}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,14 +551,14 @@
         <v>5</v>
       </c>
       <c r="G2" s="3">
-        <v>0.76180555555555562</v>
+        <v>0.3125</v>
       </c>
       <c r="H2" s="4">
-        <v>0.82500000000000007</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="I2" s="2">
         <f>HOUR(H2-G2)*60 + MINUTE(H2-G2)</f>
-        <v>91</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -652,12 +661,23 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B12" s="2">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <f>SUBTOTAL(109,Table1[Time])</f>
-        <v>695</v>
+        <v>821</v>
       </c>
     </row>
   </sheetData>
@@ -673,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA55D96-8673-42E1-9C36-AF4E023AC519}">
   <dimension ref="A3:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +750,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44003</v>
+        <v>44368</v>
       </c>
       <c r="B7" s="2">
         <v>30</v>
@@ -740,12 +760,26 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B8" s="2">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B9" s="2">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -753,7 +787,7 @@
       </c>
       <c r="B10" s="2">
         <f>SUBTOTAL(109,Table13[Time])</f>
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>